<commit_message>
LSTM, Random Forest implementation for AutoML and results
</commit_message>
<xml_diff>
--- a/results/xgboost/xgboost_tables.xlsx
+++ b/results/xgboost/xgboost_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z003t8hn\code\ML\ML-Load-Forecasting\results\xgboost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\code\ML-Load-Forecasting\results\xgboost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7645163-1A4F-4CC8-8F86-1DEDEAC0D51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3DCB4E-51CA-4562-98D9-F648AB9E4828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{EFF809F8-C2AC-43A2-A5C4-9007C01CFD9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EFF809F8-C2AC-43A2-A5C4-9007C01CFD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>colsample_bytree</t>
   </si>
@@ -69,6 +61,21 @@
   </si>
   <si>
     <t>Total parameters</t>
+  </si>
+  <si>
+    <t>XpOLJXtn</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>duration (hours)</t>
+  </si>
+  <si>
+    <t>trials</t>
+  </si>
+  <si>
+    <t>best result</t>
   </si>
 </sst>
 </file>
@@ -112,12 +119,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC115318-492C-48D0-A64A-48E4CC8F9D20}">
-  <dimension ref="F6:K16"/>
+  <dimension ref="F6:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F21" sqref="F21:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +616,42 @@
         <v>34</v>
       </c>
     </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="6">
+        <f>H22*24</f>
+        <v>23.516666666666666</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.97986111111111107</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24">
+        <v>0.96194299999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>